<commit_message>
Add OSI 2021 December account reconciliation
</commit_message>
<xml_diff>
--- a/OSI/General Journal.xlsx
+++ b/OSI/General Journal.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24827"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\pc\Dokumenter\PhD\OSI\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E13C53AD-8D3A-471E-8CA6-B23613067387}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="811"/>
+    <workbookView xWindow="4230" yWindow="2820" windowWidth="28800" windowHeight="15435" tabRatio="811" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General Journal" sheetId="2" r:id="rId1"/>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="63">
   <si>
     <t>Bilagsnr</t>
   </si>
@@ -172,12 +173,48 @@
   </si>
   <si>
     <t>Treningsavgift oktober</t>
+  </si>
+  <si>
+    <t>Vipps salg (november 2021)</t>
+  </si>
+  <si>
+    <t>Vipps salg (desember 2021)</t>
+  </si>
+  <si>
+    <t>Treningsavgift november</t>
+  </si>
+  <si>
+    <t>Diverse</t>
+  </si>
+  <si>
+    <t>Idrettsmateriell/Utstyr til eget bruk</t>
+  </si>
+  <si>
+    <t>Nytt svømmeutstyr</t>
+  </si>
+  <si>
+    <t>100 x 50m</t>
+  </si>
+  <si>
+    <t>Julebord sjokolade</t>
+  </si>
+  <si>
+    <t>refusjon</t>
+  </si>
+  <si>
+    <t>Trykksaker</t>
+  </si>
+  <si>
+    <t>Møte, kurs, oppdatering</t>
+  </si>
+  <si>
+    <t>Foodora gavekort</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="_-[$kr-414]\ * #,##0_-;\-[$kr-414]\ * #,##0_-;_-[$kr-414]\ * &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="165" formatCode="[$-414]d/\ mmm\.\ yyyy;@"/>
@@ -221,7 +258,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -231,6 +268,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -256,7 +299,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -331,6 +374,12 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -612,12 +661,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AC74"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:AC113"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G66" sqref="G66"/>
+      <pane ySplit="1" topLeftCell="A89" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C102" sqref="C102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1717,7 +1766,508 @@
       </c>
     </row>
     <row r="74" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="C74" s="2"/>
+      <c r="A74" s="11">
+        <v>44538</v>
+      </c>
+      <c r="B74" s="8">
+        <v>4990</v>
+      </c>
+      <c r="C74" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D74" s="24">
+        <v>243.74</v>
+      </c>
+      <c r="F74" s="9">
+        <v>36053</v>
+      </c>
+      <c r="G74" s="25">
+        <v>44538</v>
+      </c>
+      <c r="H74" s="9">
+        <v>21</v>
+      </c>
+      <c r="I74" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="J74" s="9">
+        <v>18</v>
+      </c>
+      <c r="L74" s="4">
+        <v>22578</v>
+      </c>
+    </row>
+    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B75" s="8">
+        <v>2410</v>
+      </c>
+      <c r="C75" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E75" s="24">
+        <v>243.74</v>
+      </c>
+    </row>
+    <row r="76" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C76" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="78" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A78" s="11">
+        <v>44543</v>
+      </c>
+      <c r="B78" s="8">
+        <v>4120</v>
+      </c>
+      <c r="C78" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D78" s="24">
+        <v>9338.7099999999991</v>
+      </c>
+      <c r="F78" s="9">
+        <v>36062</v>
+      </c>
+      <c r="G78" s="25">
+        <v>44543</v>
+      </c>
+      <c r="H78" s="9">
+        <v>21</v>
+      </c>
+      <c r="I78" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="J78" s="9">
+        <v>18</v>
+      </c>
+      <c r="L78" s="4">
+        <v>22605</v>
+      </c>
+    </row>
+    <row r="79" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B79" s="8">
+        <v>2410</v>
+      </c>
+      <c r="C79" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E79" s="24">
+        <v>9338.7099999999991</v>
+      </c>
+    </row>
+    <row r="80" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C80" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="82" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A82" s="11">
+        <v>44544</v>
+      </c>
+      <c r="B82" s="8">
+        <v>6860</v>
+      </c>
+      <c r="C82" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D82" s="24">
+        <v>1500</v>
+      </c>
+      <c r="F82" s="9">
+        <v>36063</v>
+      </c>
+      <c r="G82" s="25">
+        <v>44544</v>
+      </c>
+      <c r="H82" s="9">
+        <v>21</v>
+      </c>
+      <c r="I82" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="J82" s="9">
+        <v>18</v>
+      </c>
+      <c r="L82" s="4">
+        <v>22612</v>
+      </c>
+    </row>
+    <row r="83" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B83" s="8">
+        <v>2410</v>
+      </c>
+      <c r="C83" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E83" s="24">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="84" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C84" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="86" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A86" s="11">
+        <v>44545</v>
+      </c>
+      <c r="B86" s="8">
+        <v>4990</v>
+      </c>
+      <c r="C86" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D86" s="24">
+        <v>238.8</v>
+      </c>
+      <c r="F86" s="9">
+        <v>36066</v>
+      </c>
+      <c r="G86" s="25">
+        <v>44545</v>
+      </c>
+      <c r="H86" s="9">
+        <v>21</v>
+      </c>
+      <c r="I86" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="J86" s="9">
+        <v>18</v>
+      </c>
+      <c r="L86" s="4">
+        <v>22643</v>
+      </c>
+    </row>
+    <row r="87" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B87" s="8">
+        <v>2410</v>
+      </c>
+      <c r="C87" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E87" s="24">
+        <v>238.8</v>
+      </c>
+    </row>
+    <row r="88" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C88" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="90" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A90" s="11">
+        <v>44550</v>
+      </c>
+      <c r="B90" s="8">
+        <v>6820</v>
+      </c>
+      <c r="C90" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D90" s="24">
+        <v>987</v>
+      </c>
+      <c r="F90" s="9">
+        <v>36117</v>
+      </c>
+      <c r="G90" s="25">
+        <v>44550</v>
+      </c>
+      <c r="H90" s="9">
+        <v>21</v>
+      </c>
+      <c r="I90" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="J90" s="9">
+        <v>18</v>
+      </c>
+      <c r="L90" s="4">
+        <v>22814</v>
+      </c>
+    </row>
+    <row r="91" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B91" s="8">
+        <v>2410</v>
+      </c>
+      <c r="C91" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E91" s="24">
+        <v>978</v>
+      </c>
+    </row>
+    <row r="93" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A93" s="11">
+        <v>44560</v>
+      </c>
+      <c r="B93" s="8">
+        <v>4990</v>
+      </c>
+      <c r="C93" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D93" s="24">
+        <v>5275</v>
+      </c>
+      <c r="F93" s="9">
+        <v>36118</v>
+      </c>
+      <c r="G93" s="25">
+        <v>44559</v>
+      </c>
+      <c r="H93" s="9">
+        <v>21</v>
+      </c>
+      <c r="I93" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="J93" s="9">
+        <v>18</v>
+      </c>
+      <c r="L93" s="4">
+        <v>22816</v>
+      </c>
+    </row>
+    <row r="94" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B94" s="8">
+        <v>2410</v>
+      </c>
+      <c r="C94" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E94" s="24">
+        <v>5275</v>
+      </c>
+    </row>
+    <row r="95" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C95" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="97" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A97" s="11">
+        <v>44596</v>
+      </c>
+      <c r="B97" s="8">
+        <v>1920</v>
+      </c>
+      <c r="C97" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D97" s="26">
+        <v>176.84</v>
+      </c>
+      <c r="F97" s="9">
+        <v>28030</v>
+      </c>
+      <c r="G97" s="25">
+        <v>44523</v>
+      </c>
+      <c r="H97" s="9">
+        <v>1</v>
+      </c>
+      <c r="I97" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="J97" s="9">
+        <v>18</v>
+      </c>
+      <c r="L97" s="4">
+        <v>22662</v>
+      </c>
+    </row>
+    <row r="98" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B98" s="8">
+        <v>7770</v>
+      </c>
+      <c r="C98" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="D98" s="24">
+        <v>3.16</v>
+      </c>
+    </row>
+    <row r="99" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B99" s="8">
+        <v>3990</v>
+      </c>
+      <c r="C99" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E99" s="24">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="100" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C100" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="102" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A102" s="11">
+        <v>44596</v>
+      </c>
+      <c r="B102" s="8">
+        <v>1920</v>
+      </c>
+      <c r="C102" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D102" s="23">
+        <v>88.42</v>
+      </c>
+      <c r="F102" s="9">
+        <v>28079</v>
+      </c>
+      <c r="G102" s="25">
+        <v>44533</v>
+      </c>
+      <c r="H102" s="9">
+        <v>1</v>
+      </c>
+      <c r="I102" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="J102" s="9">
+        <v>18</v>
+      </c>
+      <c r="L102" s="4">
+        <v>22937</v>
+      </c>
+    </row>
+    <row r="103" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B103" s="8">
+        <v>7770</v>
+      </c>
+      <c r="C103" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="D103" s="24">
+        <v>1.58</v>
+      </c>
+    </row>
+    <row r="104" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B104" s="8">
+        <v>3990</v>
+      </c>
+      <c r="C104" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E104" s="24">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="105" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C105" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="107" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A107" s="11">
+        <v>44596</v>
+      </c>
+      <c r="B107" s="8">
+        <v>1510</v>
+      </c>
+      <c r="C107" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D107" s="23">
+        <v>90</v>
+      </c>
+      <c r="E107" s="23"/>
+    </row>
+    <row r="108" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B108" s="8">
+        <v>3920</v>
+      </c>
+      <c r="C108" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D108" s="23"/>
+      <c r="E108" s="23">
+        <v>90</v>
+      </c>
+      <c r="F108" s="9">
+        <v>60017</v>
+      </c>
+      <c r="G108" s="25">
+        <v>44530</v>
+      </c>
+      <c r="H108" s="9">
+        <v>2</v>
+      </c>
+      <c r="I108" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="J108" s="9">
+        <v>18</v>
+      </c>
+      <c r="K108" s="9">
+        <v>9</v>
+      </c>
+      <c r="L108" s="4">
+        <v>22865</v>
+      </c>
+    </row>
+    <row r="109" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C109" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D109" s="23"/>
+      <c r="E109" s="23"/>
+    </row>
+    <row r="111" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A111" s="11">
+        <v>44596</v>
+      </c>
+      <c r="B111" s="8">
+        <v>4200</v>
+      </c>
+      <c r="C111" s="27" t="s">
+        <v>39</v>
+      </c>
+      <c r="D111" s="24">
+        <v>1000</v>
+      </c>
+      <c r="F111" s="9">
+        <v>36097</v>
+      </c>
+      <c r="G111" s="25">
+        <v>44550</v>
+      </c>
+      <c r="H111" s="9">
+        <v>21</v>
+      </c>
+      <c r="I111" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="J111" s="9">
+        <v>18</v>
+      </c>
+      <c r="L111" s="4">
+        <v>22656</v>
+      </c>
+    </row>
+    <row r="112" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B112" s="8">
+        <v>2410</v>
+      </c>
+      <c r="C112" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E112" s="24">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="113" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C113" s="2" t="s">
+        <v>7</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Rearrange OSI folder such that 2021 files stay together
</commit_message>
<xml_diff>
--- a/OSI/General Journal.xlsx
+++ b/OSI/General Journal.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\pc\Dokumenter\PhD\OSI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E13C53AD-8D3A-471E-8CA6-B23613067387}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5467689-7460-4030-930C-ABABC2BA09EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4230" yWindow="2820" windowWidth="28800" windowHeight="15435" tabRatio="811" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2892" yWindow="1152" windowWidth="17280" windowHeight="8964" tabRatio="811" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General Journal" sheetId="2" r:id="rId1"/>
@@ -665,27 +665,27 @@
   <dimension ref="A1:AC113"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A89" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C102" sqref="C102"/>
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.140625" style="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.7109375" style="8" customWidth="1"/>
-    <col min="3" max="3" width="59.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="11.7109375" style="24" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.140625" style="9" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.5703125" style="9" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="25.7109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="9.140625" style="9"/>
-    <col min="12" max="12" width="9.140625" style="4"/>
-    <col min="13" max="29" width="9.140625" style="21"/>
-    <col min="30" max="16384" width="9.140625" style="7"/>
+    <col min="1" max="1" width="13.109375" style="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.6640625" style="8" customWidth="1"/>
+    <col min="3" max="3" width="59.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="11.6640625" style="24" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.5546875" style="9" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="25.6640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="9.109375" style="9"/>
+    <col min="12" max="12" width="9.109375" style="4"/>
+    <col min="13" max="29" width="9.109375" style="21"/>
+    <col min="30" max="16384" width="9.109375" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" s="13" customFormat="1" ht="28.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:29" s="13" customFormat="1" ht="28.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="15" t="s">
         <v>2</v>
       </c>
@@ -740,7 +740,7 @@
       <c r="AB1" s="6"/>
       <c r="AC1" s="6"/>
     </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A2" s="11">
         <v>44229</v>
       </c>
@@ -773,7 +773,7 @@
         <v>20264</v>
       </c>
     </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:29" x14ac:dyDescent="0.3">
       <c r="B3" s="8">
         <v>2410</v>
       </c>
@@ -786,7 +786,7 @@
       </c>
       <c r="G3" s="10"/>
     </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:29" x14ac:dyDescent="0.3">
       <c r="C4" s="2" t="s">
         <v>7</v>
       </c>
@@ -794,12 +794,12 @@
       <c r="E4" s="23"/>
       <c r="G4" s="10"/>
     </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:29" x14ac:dyDescent="0.3">
       <c r="D5" s="23"/>
       <c r="E5" s="23"/>
       <c r="G5" s="10"/>
     </row>
-    <row r="6" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A6" s="11">
         <v>44237</v>
       </c>
@@ -814,7 +814,7 @@
       </c>
       <c r="E6" s="23"/>
     </row>
-    <row r="7" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:29" x14ac:dyDescent="0.3">
       <c r="B7" s="8">
         <v>3480</v>
       </c>
@@ -847,7 +847,7 @@
         <v>20405</v>
       </c>
     </row>
-    <row r="8" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:29" x14ac:dyDescent="0.3">
       <c r="C8" s="2" t="s">
         <v>9</v>
       </c>
@@ -855,14 +855,14 @@
       <c r="E8" s="23"/>
       <c r="G8" s="10"/>
     </row>
-    <row r="9" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:29" x14ac:dyDescent="0.3">
       <c r="B9" s="12"/>
       <c r="C9" s="7"/>
       <c r="D9" s="23"/>
       <c r="E9" s="23"/>
       <c r="G9" s="10"/>
     </row>
-    <row r="10" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A10" s="11">
         <v>44281</v>
       </c>
@@ -878,7 +878,7 @@
       <c r="E10" s="23"/>
       <c r="G10" s="10"/>
     </row>
-    <row r="11" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:29" x14ac:dyDescent="0.3">
       <c r="B11" s="8">
         <v>3920</v>
       </c>
@@ -908,7 +908,7 @@
         <v>20515</v>
       </c>
     </row>
-    <row r="12" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:29" x14ac:dyDescent="0.3">
       <c r="C12" s="2" t="s">
         <v>20</v>
       </c>
@@ -916,12 +916,12 @@
       <c r="E12" s="23"/>
       <c r="G12" s="10"/>
     </row>
-    <row r="13" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:29" x14ac:dyDescent="0.3">
       <c r="D13" s="23"/>
       <c r="E13" s="23"/>
       <c r="G13" s="10"/>
     </row>
-    <row r="14" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:29" x14ac:dyDescent="0.3">
       <c r="A14" s="11">
         <v>44312</v>
       </c>
@@ -936,7 +936,7 @@
       </c>
       <c r="E14" s="23"/>
     </row>
-    <row r="15" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:29" x14ac:dyDescent="0.3">
       <c r="B15" s="8">
         <v>3480</v>
       </c>
@@ -969,7 +969,7 @@
         <v>20654</v>
       </c>
     </row>
-    <row r="16" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:29" x14ac:dyDescent="0.3">
       <c r="C16" s="2" t="s">
         <v>18</v>
       </c>
@@ -977,12 +977,12 @@
       <c r="E16" s="23"/>
       <c r="G16" s="10"/>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="D17" s="23"/>
       <c r="E17" s="23"/>
       <c r="G17" s="10"/>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A18" s="11">
         <v>44397</v>
       </c>
@@ -1014,7 +1014,7 @@
         <v>21037</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B19" s="8">
         <v>2410</v>
       </c>
@@ -1026,17 +1026,17 @@
       </c>
       <c r="G19" s="10"/>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C20" s="2" t="s">
         <v>35</v>
       </c>
       <c r="G20" s="10"/>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C21" s="2"/>
       <c r="G21" s="10"/>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A22" s="11">
         <v>44432</v>
       </c>
@@ -1068,7 +1068,7 @@
         <v>21161</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B23" s="8">
         <v>4990</v>
       </c>
@@ -1080,7 +1080,7 @@
       </c>
       <c r="G23" s="10"/>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B24" s="8">
         <v>2410</v>
       </c>
@@ -1092,17 +1092,17 @@
       </c>
       <c r="G24" s="10"/>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C25" s="2" t="s">
         <v>32</v>
       </c>
       <c r="G25" s="10"/>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C26" s="2"/>
       <c r="G26" s="10"/>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A27" s="11">
         <v>44453</v>
       </c>
@@ -1117,7 +1117,7 @@
       </c>
       <c r="E27" s="23"/>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B28" s="8">
         <v>3920</v>
       </c>
@@ -1150,7 +1150,7 @@
         <v>21130</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C29" s="2" t="s">
         <v>42</v>
       </c>
@@ -1158,12 +1158,12 @@
       <c r="E29" s="23"/>
       <c r="G29" s="10"/>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
       <c r="D30" s="23"/>
       <c r="E30" s="23"/>
       <c r="G30" s="10"/>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A31" s="11">
         <v>44453</v>
       </c>
@@ -1178,7 +1178,7 @@
       </c>
       <c r="E31" s="23"/>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B32" s="8">
         <v>3920</v>
       </c>
@@ -1211,7 +1211,7 @@
         <v>21129</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C33" s="2" t="s">
         <v>43</v>
       </c>
@@ -1219,13 +1219,13 @@
       <c r="E33" s="23"/>
       <c r="G33" s="10"/>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C34" s="2"/>
       <c r="D34" s="23"/>
       <c r="E34" s="23"/>
       <c r="G34" s="10"/>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A35" s="11">
         <v>44464</v>
       </c>
@@ -1257,7 +1257,7 @@
         <v>21415</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B36" s="8">
         <v>2410</v>
       </c>
@@ -1269,17 +1269,17 @@
       </c>
       <c r="G36" s="10"/>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C37" s="2" t="s">
         <v>33</v>
       </c>
       <c r="G37" s="10"/>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C38" s="2"/>
       <c r="G38" s="10"/>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A39" s="11">
         <v>44468</v>
       </c>
@@ -1311,7 +1311,7 @@
         <v>21509</v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B40" s="8">
         <v>2410</v>
       </c>
@@ -1323,17 +1323,17 @@
       </c>
       <c r="G40" s="10"/>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C41" s="2" t="s">
         <v>46</v>
       </c>
       <c r="G41" s="10"/>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C42" s="2"/>
       <c r="G42" s="10"/>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A43" s="11">
         <v>44480</v>
       </c>
@@ -1365,7 +1365,7 @@
         <v>21748</v>
       </c>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B44" s="8">
         <v>2410</v>
       </c>
@@ -1376,15 +1376,15 @@
         <v>9100</v>
       </c>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C45" s="2" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C46" s="2"/>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A47" s="11">
         <v>44505</v>
       </c>
@@ -1400,7 +1400,7 @@
       <c r="E47" s="23"/>
       <c r="G47" s="10"/>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B48" s="8">
         <v>3920</v>
       </c>
@@ -1433,7 +1433,7 @@
         <v>21745</v>
       </c>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C49" s="2" t="s">
         <v>44</v>
       </c>
@@ -1441,12 +1441,12 @@
       <c r="E49" s="23"/>
       <c r="G49" s="10"/>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.3">
       <c r="D50" s="23"/>
       <c r="E50" s="23"/>
       <c r="G50" s="10"/>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A51" s="11">
         <v>44505</v>
       </c>
@@ -1462,7 +1462,7 @@
       <c r="E51" s="23"/>
       <c r="G51" s="10"/>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B52" s="12">
         <v>7770</v>
       </c>
@@ -1475,7 +1475,7 @@
       <c r="E52" s="23"/>
       <c r="G52" s="10"/>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B53" s="8">
         <v>3990</v>
       </c>
@@ -1505,7 +1505,7 @@
         <v>21686</v>
       </c>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C54" s="2" t="s">
         <v>47</v>
       </c>
@@ -1513,13 +1513,13 @@
       <c r="E54" s="23"/>
       <c r="G54" s="10"/>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C55" s="2"/>
       <c r="D55" s="23"/>
       <c r="E55" s="23"/>
       <c r="G55" s="10"/>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A56" s="11">
         <v>44505</v>
       </c>
@@ -1535,7 +1535,7 @@
       <c r="E56" s="23"/>
       <c r="G56" s="10"/>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B57" s="8">
         <v>3920</v>
       </c>
@@ -1568,7 +1568,7 @@
         <v>21746</v>
       </c>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C58" s="2" t="s">
         <v>45</v>
       </c>
@@ -1576,11 +1576,11 @@
       <c r="E58" s="23"/>
       <c r="G58" s="10"/>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C59" s="2"/>
       <c r="G59" s="10"/>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A60" s="11">
         <v>44505</v>
       </c>
@@ -1595,7 +1595,7 @@
       </c>
       <c r="G60" s="10"/>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B61" s="12">
         <v>7770</v>
       </c>
@@ -1607,7 +1607,7 @@
       </c>
       <c r="G61" s="10"/>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B62" s="8">
         <v>3990</v>
       </c>
@@ -1636,17 +1636,17 @@
         <v>21765</v>
       </c>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C63" s="2" t="s">
         <v>48</v>
       </c>
       <c r="G63" s="10"/>
     </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C64" s="2"/>
       <c r="G64" s="10"/>
     </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A65" s="11">
         <v>44526</v>
       </c>
@@ -1661,7 +1661,7 @@
       </c>
       <c r="E65" s="23"/>
     </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B66" s="8">
         <v>3920</v>
       </c>
@@ -1694,18 +1694,18 @@
         <v>22338</v>
       </c>
     </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C67" s="2" t="s">
         <v>50</v>
       </c>
       <c r="D67" s="23"/>
       <c r="E67" s="23"/>
     </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C68" s="2"/>
       <c r="G68" s="10"/>
     </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A69" s="11">
         <v>44526</v>
       </c>
@@ -1720,7 +1720,7 @@
       </c>
       <c r="G69" s="10"/>
     </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B70" s="12">
         <v>7770</v>
       </c>
@@ -1731,7 +1731,7 @@
         <v>17.59</v>
       </c>
     </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B71" s="8">
         <v>3990</v>
       </c>
@@ -1760,12 +1760,12 @@
         <v>22366</v>
       </c>
     </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C72" s="2" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A74" s="11">
         <v>44538</v>
       </c>
@@ -1797,7 +1797,7 @@
         <v>22578</v>
       </c>
     </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B75" s="8">
         <v>2410</v>
       </c>
@@ -1808,12 +1808,12 @@
         <v>243.74</v>
       </c>
     </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C76" s="2" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A78" s="11">
         <v>44543</v>
       </c>
@@ -1845,7 +1845,7 @@
         <v>22605</v>
       </c>
     </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B79" s="8">
         <v>2410</v>
       </c>
@@ -1856,12 +1856,12 @@
         <v>9338.7099999999991</v>
       </c>
     </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C80" s="2" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="82" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A82" s="11">
         <v>44544</v>
       </c>
@@ -1893,7 +1893,7 @@
         <v>22612</v>
       </c>
     </row>
-    <row r="83" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B83" s="8">
         <v>2410</v>
       </c>
@@ -1904,12 +1904,12 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="84" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C84" s="2" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="86" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A86" s="11">
         <v>44545</v>
       </c>
@@ -1941,7 +1941,7 @@
         <v>22643</v>
       </c>
     </row>
-    <row r="87" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B87" s="8">
         <v>2410</v>
       </c>
@@ -1952,12 +1952,12 @@
         <v>238.8</v>
       </c>
     </row>
-    <row r="88" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C88" s="2" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="90" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A90" s="11">
         <v>44550</v>
       </c>
@@ -1989,7 +1989,7 @@
         <v>22814</v>
       </c>
     </row>
-    <row r="91" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B91" s="8">
         <v>2410</v>
       </c>
@@ -2000,7 +2000,7 @@
         <v>978</v>
       </c>
     </row>
-    <row r="93" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A93" s="11">
         <v>44560</v>
       </c>
@@ -2032,7 +2032,7 @@
         <v>22816</v>
       </c>
     </row>
-    <row r="94" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B94" s="8">
         <v>2410</v>
       </c>
@@ -2043,12 +2043,12 @@
         <v>5275</v>
       </c>
     </row>
-    <row r="95" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C95" s="2" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="97" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A97" s="11">
         <v>44596</v>
       </c>
@@ -2080,7 +2080,7 @@
         <v>22662</v>
       </c>
     </row>
-    <row r="98" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B98" s="8">
         <v>7770</v>
       </c>
@@ -2091,7 +2091,7 @@
         <v>3.16</v>
       </c>
     </row>
-    <row r="99" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B99" s="8">
         <v>3990</v>
       </c>
@@ -2102,12 +2102,12 @@
         <v>180</v>
       </c>
     </row>
-    <row r="100" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C100" s="2" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="102" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A102" s="11">
         <v>44596</v>
       </c>
@@ -2139,7 +2139,7 @@
         <v>22937</v>
       </c>
     </row>
-    <row r="103" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B103" s="8">
         <v>7770</v>
       </c>
@@ -2150,7 +2150,7 @@
         <v>1.58</v>
       </c>
     </row>
-    <row r="104" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B104" s="8">
         <v>3990</v>
       </c>
@@ -2161,12 +2161,12 @@
         <v>90</v>
       </c>
     </row>
-    <row r="105" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C105" s="2" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="107" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A107" s="11">
         <v>44596</v>
       </c>
@@ -2181,7 +2181,7 @@
       </c>
       <c r="E107" s="23"/>
     </row>
-    <row r="108" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B108" s="8">
         <v>3920</v>
       </c>
@@ -2214,14 +2214,14 @@
         <v>22865</v>
       </c>
     </row>
-    <row r="109" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:12" x14ac:dyDescent="0.3">
       <c r="C109" s="2" t="s">
         <v>53</v>
       </c>
       <c r="D109" s="23"/>
       <c r="E109" s="23"/>
     </row>
-    <row r="111" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A111" s="11">
         <v>44596</v>
       </c>
@@ -2253,7 +2253,7 @@
         <v>22656</v>
       </c>
     </row>
-    <row r="112" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B112" s="8">
         <v>2410</v>
       </c>
@@ -2264,7 +2264,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="113" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="113" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C113" s="2" t="s">
         <v>7</v>
       </c>

</xml_diff>